<commit_message>
Oudoor plants' locations, Excel sheets updates
</commit_message>
<xml_diff>
--- a/data/Creators.xlsx
+++ b/data/Creators.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29602"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="118" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5C6D6409-49BA-4391-8ED7-D7335EB1792F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4BD9966A-7B49-4E7F-8CBB-B10FC3E0D003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="32">
   <si>
     <t>Creator type</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>Eman Kamal Ajaj</t>
+  </si>
+  <si>
+    <t>Saleh Ahmed Saleh</t>
   </si>
   <si>
     <t>Software Engineer</t>
@@ -498,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C64"/>
+  <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -757,16 +760,16 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="C25" s="1"/>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>30</v>
@@ -774,8 +777,12 @@
       <c r="C26" s="1"/>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
+      <c r="A27" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="C27" s="1"/>
     </row>
     <row r="28" spans="1:3">
@@ -963,9 +970,14 @@
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
     </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A100" xr:uid="{B6AF7961-A03A-4E2D-83CF-3B93FCCC5772}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A101" xr:uid="{B6AF7961-A03A-4E2D-83CF-3B93FCCC5772}">
       <formula1>"Software Engineer, Landscape Engineer, Biologist"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>